<commit_message>
set foundation for most existing Freemotion...
</commit_message>
<xml_diff>
--- a/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
+++ b/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\specsheetsConsole\Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan.lee\Documents\GitHub\LabVIEW\Projects\1259_usbComm\specsheetsConsole\Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2222,23 +2222,6 @@
 Turn on TV with console controls and play video source on TV
 Audio will play through the console speakers
 Adjust TV audio volume on console and the function will display on the TV and the console audio will reflect change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">将音频源连接到EQF1293并按播放
-将EQWxxxx公头直流电连接到公头直流电源适配器电缆，连接到EQF1293和控制台的其他端到端
-将RJ45以太网电缆的一端连接到EQF1293和控制台的另一端到后端
-将耳机连接到控制台并放在耳朵上
-按下控制台上的所有电视控制按钮，EQF1293上将显示响应
-音频将通过耳机播放
-在控制台上调整电视音频音量，该功能将显示在MYE电视上，耳机音频将反映变化 
-Connect audio source to EQF1293 and press play
-Connect EQWxxxx male dc to male dc power adapter cable to EQF1293 and other end to back of console
-Connect one end of RJ45 ethernet cable to the EQF1293 and other end to back of console
-Connect headphones to console and place on ears
-Press all the TV control buttons on the console and a response will appear on the EQF1293
-Audio will play through the headphones
-Adjust TV audio volume on console and the function will display on the MYE TV and the headphone audio will reflect change
-</t>
   </si>
   <si>
     <t>将RJ45以太网电缆的一端连接到MYE CardioCare，另一端连接到控制台的背面
@@ -3029,20 +3012,6 @@
 On audio device, enter the bluetooth setup screen and disconnect and unpair ifit Audio.</t>
   </si>
   <si>
-    <t>将EQF1007的一端连接到音频源，另一端连接到MYE音频发送器。
-打开MYE音频发射器电源并播放音频源。
-将耳机连接到控制台。
-将MYE音频接收器连接至控制台背面的RJ45电缆。
-音频源将通过耳机播放。
-调节音量，耳机音频将反映变化。
-Connect one end of EQF1007 to audio source and the other end to MYE audio transmitter.
-Power up MYE audio transmitter and play audio source.
-Connect headphones to console.
-Connect MYE audio receiver to RJ45 cable on the back of console.
-Audio source will play through the headphones.
-Adjust volume and the headphone audio will reflect change.</t>
-  </si>
-  <si>
     <t>触摸屏幕右下角的用户个人资料图标，清除缓存。
 触摸设置。
 触摸维护。
@@ -3161,6 +3130,32 @@
 On the console, press the Large Fan button to turn fan on. Fan should run on low.
 Press the Large Fan button again until is on high.
 Press the Small Fan button until it turns the fan off.</t>
+  </si>
+  <si>
+    <t>将EQF1007的一端连接到音频源，另一端连接到MYE音频发送器。
+打开MYE音频发射器电源并播放音频源。
+将耳机连接到控制台。
+将MYE音频接收器连接至控制台背面的RJ45电缆。
+音频源将通过耳机播放。
+调节音量，耳机音频将反映变化。
+Connect audio source to EQF1293 and press play
+Connect EQWxxxx male dc to male dc power adapter cable to EQF1293 and other end to back of console
+Connect one end of RJ45 ethernet cable to the EQF1293 and other end to back of console
+Connect headphones to console and place on ears
+Audio source will play through the headphones.
+Adjust volume and the headphone audio will reflect change.</t>
+  </si>
+  <si>
+    <t>将音频源连接到EQF1293并按播放
+将EQWxxxx公头直流电连接到公头直流电源适配器电缆，连接到EQF1293和控制台的其他端到端
+将RJ45以太网电缆的一端连接到EQF1293和控制台的另一端到后端
+将耳机连接到控制台并放在耳朵上
+按下控制台上的所有电视控制按钮，EQF1293上将显示响应
+音频将通过耳机播放
+在控制台上调整电视音频音量，该功能将显示在MYE电视上，耳机音频将反映变化 
+Connect EQWxxxx male dc to male dc power adapter cable to EQF1293 and other end to back of console
+Connect one end of RJ45 ethernet cable to the EQF1293 and other end to back of console
+Press all the TV control buttons on the console and a response will appear on the EQF1293</t>
   </si>
 </sst>
 </file>
@@ -3532,8 +3527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3543,82 +3538,82 @@
   <sheetData>
     <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>381</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>382</v>
       </c>
       <c r="Y1" s="6">
         <v>-24</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AA1" s="6"/>
     </row>
@@ -3627,10 +3622,10 @@
         <v>319</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>337</v>
@@ -3639,25 +3634,25 @@
         <v>338</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>340</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>341</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>343</v>
@@ -3672,31 +3667,31 @@
         <v>347</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T2" s="5" t="s">
         <v>348</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="V2" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="W2" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="W2" s="5" t="s">
-        <v>352</v>
-      </c>
       <c r="X2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3704,10 +3699,10 @@
         <v>320</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
@@ -3716,25 +3711,25 @@
         <v>339</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>431</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>345</v>
@@ -3746,16 +3741,16 @@
         <v>4</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>349</v>
@@ -3778,7 +3773,7 @@
         <v>321</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -3790,7 +3785,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>4</v>
@@ -3799,22 +3794,22 @@
         <v>4</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>350</v>
+        <v>467</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>4</v>
@@ -3826,7 +3821,7 @@
         <v>4</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3834,7 +3829,7 @@
         <v>322</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>4</v>
@@ -3846,7 +3841,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>4</v>
@@ -3855,25 +3850,25 @@
         <v>4</v>
       </c>
       <c r="I5" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>432</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>433</v>
-      </c>
       <c r="K5" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>436</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>437</v>
-      </c>
       <c r="R5" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>455</v>
+        <v>466</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>4</v>
@@ -3888,7 +3883,7 @@
         <v>4</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3896,7 +3891,7 @@
         <v>323</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>4</v>
@@ -3917,25 +3912,25 @@
         <v>4</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="N6" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>460</v>
       </c>
-      <c r="O6" s="5" t="s">
-        <v>462</v>
-      </c>
       <c r="P6" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>4</v>
@@ -3956,7 +3951,7 @@
         <v>4</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -3964,7 +3959,7 @@
         <v>324</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -3976,7 +3971,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>4</v>
@@ -3985,13 +3980,13 @@
         <v>4</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>4</v>
@@ -4032,7 +4027,7 @@
         <v>325</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -4044,7 +4039,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>4</v>
@@ -4053,10 +4048,10 @@
         <v>4</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>342</v>
@@ -4103,7 +4098,7 @@
         <v>325</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -4115,7 +4110,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>4</v>
@@ -4124,13 +4119,13 @@
         <v>4</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>4</v>
@@ -4177,7 +4172,7 @@
         <v>326</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -4189,7 +4184,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>4</v>
@@ -4198,7 +4193,7 @@
         <v>4</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>4</v>
@@ -4242,10 +4237,10 @@
     </row>
     <row r="11" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
@@ -4257,7 +4252,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>4</v>
@@ -4266,13 +4261,13 @@
         <v>4</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>4</v>
@@ -4319,7 +4314,7 @@
         <v>327</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>4</v>
@@ -4396,7 +4391,7 @@
         <v>328</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>4</v>
@@ -4417,10 +4412,10 @@
         <v>4</v>
       </c>
       <c r="I13" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="K13" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>444</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>4</v>
@@ -4467,7 +4462,7 @@
         <v>329</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>4</v>
@@ -4544,7 +4539,7 @@
         <v>330</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>4</v>
@@ -4621,7 +4616,7 @@
         <v>331</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>4</v>
@@ -4633,7 +4628,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>4</v>
@@ -4698,7 +4693,7 @@
         <v>332</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>4</v>
@@ -4710,7 +4705,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>4</v>
@@ -4775,7 +4770,7 @@
         <v>333</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>4</v>
@@ -4787,7 +4782,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>4</v>
@@ -4852,7 +4847,7 @@
         <v>334</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -4864,7 +4859,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>4</v>
@@ -4929,7 +4924,7 @@
         <v>335</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
@@ -4941,7 +4936,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>4</v>
@@ -5006,7 +5001,7 @@
         <v>336</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>4</v>
@@ -5080,7 +5075,7 @@
     </row>
     <row r="22" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
@@ -10087,13 +10082,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B1" s="3">
         <v>20191212</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
@@ -10101,13 +10096,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B2" s="3">
         <v>20191205</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Working on database issues
</commit_message>
<xml_diff>
--- a/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
+++ b/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="466">
   <si>
     <t>Rev0</t>
   </si>
@@ -2039,38 +2039,6 @@
 </t>
   </si>
   <si>
-    <t>EQF1259控制台夹具
-PC w /访问RNDftp
-MicroSD卡
-EQF1259 Console Fixture
-PC w/ Access to RNDftp
-MicroSD Card</t>
-  </si>
-  <si>
-    <t>EQW1141; 2针线束 
-EQW1141; 2-pin harness</t>
-  </si>
-  <si>
-    <t>EQW1011; 3针线束 
-EQW1011; 3-pin harness</t>
-  </si>
-  <si>
-    <t>EQW1059; 4针线束 
-EQW1059; 4-pin harness</t>
-  </si>
-  <si>
-    <t>EQW1067; 5针线束 
-EQW1067; 5-pin harness</t>
-  </si>
-  <si>
-    <t>EQW1001; 8针线束 
-EQW1001; 8-pin harness</t>
-  </si>
-  <si>
-    <t>EQW1139; 10针线束 
-EQW1139; 10-pin harness</t>
-  </si>
-  <si>
     <t>EQW1053; 14针线束 
 EQW1053; 14-pin harness</t>
   </si>
@@ -2263,9 +2231,6 @@
   </si>
   <si>
     <t>EQUIPMENT_NEEDED-0</t>
-  </si>
-  <si>
-    <t>FIXTURE_SETUP-1</t>
   </si>
   <si>
     <t>BLE_SETUP-2</t>
@@ -3129,6 +3094,45 @@
 Connect EQWxxxx male dc to male dc power adapter cable to EQF1293 and other end to back of console
 Connect one end of RJ45 ethernet cable to the EQF1293 and other end to back of console
 On the console, connect headphones and adjust volume to minimum and maximum and verify a change.</t>
+  </si>
+  <si>
+    <t>FIXTURE_SETUP-1</t>
+  </si>
+  <si>
+    <t>EQW1141； 2针线束
+EQW1141; 2-pin harness</t>
+  </si>
+  <si>
+    <t>EQW1011； 3针线束
+EQW1011; 3-pin harness</t>
+  </si>
+  <si>
+    <t>EQW1059； 4针线束
+EQW1059; 4-pin harness</t>
+  </si>
+  <si>
+    <t>EQW1067； 5针线束
+EQW1067; 5-pin harness</t>
+  </si>
+  <si>
+    <t>EQW1001； 8针线束
+EQW1001; 8-pin harness</t>
+  </si>
+  <si>
+    <t>EQW1139； 10针线束
+EQW1139; 10-pin harness</t>
+  </si>
+  <si>
+    <t>EQW1025； 12针线束
+EQW1025; 12-pin harness</t>
+  </si>
+  <si>
+    <t>EQF1259控制台装置
+带有/访问ANDftp的PC
+MicroSD卡
+EQF1259 Console Fixture
+PC w/ Access to RNDftp
+MicroSD Card</t>
   </si>
 </sst>
 </file>
@@ -3500,8 +3504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3511,70 +3515,70 @@
   <sheetData>
     <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>369</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>371</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>373</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>374</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>377</v>
       </c>
       <c r="W1" s="6">
         <v>-22</v>
@@ -3586,123 +3590,123 @@
         <v>-24</v>
       </c>
       <c r="Z1" s="6" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="AA1" s="6"/>
     </row>
     <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>319</v>
+        <v>465</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>418</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>413</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>337</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="O2" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>421</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>457</v>
-      </c>
       <c r="S2" s="5" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="V2" s="5" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>320</v>
+        <v>458</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>414</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>448</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>422</v>
-      </c>
       <c r="K3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="O3" s="5" t="s">
         <v>4</v>
@@ -3711,19 +3715,19 @@
         <v>4</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="V3" s="5" t="s">
         <v>4</v>
@@ -3740,10 +3744,10 @@
     </row>
     <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>321</v>
+        <v>459</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -3755,7 +3759,7 @@
         <v>4</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>4</v>
@@ -3764,22 +3768,22 @@
         <v>4</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>4</v>
@@ -3791,15 +3795,15 @@
         <v>4</v>
       </c>
       <c r="Z4" s="5" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>322</v>
+        <v>460</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>4</v>
@@ -3811,7 +3815,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>4</v>
@@ -3820,25 +3824,25 @@
         <v>4</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>4</v>
@@ -3853,15 +3857,15 @@
         <v>4</v>
       </c>
       <c r="Z5" s="5" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>323</v>
+        <v>461</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>4</v>
@@ -3882,25 +3886,25 @@
         <v>4</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>4</v>
@@ -3921,15 +3925,15 @@
         <v>4</v>
       </c>
       <c r="Z6" s="5" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>324</v>
+        <v>462</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -3941,7 +3945,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>4</v>
@@ -3950,13 +3954,13 @@
         <v>4</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>4</v>
@@ -3994,10 +3998,10 @@
     </row>
     <row r="8" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>325</v>
+        <v>463</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -4009,7 +4013,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>4</v>
@@ -4018,13 +4022,13 @@
         <v>4</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="M8" s="5" t="s">
         <v>4</v>
@@ -4065,10 +4069,10 @@
     </row>
     <row r="9" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>325</v>
+        <v>464</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -4080,7 +4084,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>4</v>
@@ -4089,13 +4093,13 @@
         <v>4</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>4</v>
@@ -4139,10 +4143,10 @@
     </row>
     <row r="10" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -4154,7 +4158,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>4</v>
@@ -4163,7 +4167,7 @@
         <v>4</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>4</v>
@@ -4207,10 +4211,10 @@
     </row>
     <row r="11" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
@@ -4222,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>4</v>
@@ -4231,13 +4235,13 @@
         <v>4</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>4</v>
@@ -4281,10 +4285,10 @@
     </row>
     <row r="12" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>4</v>
@@ -4358,10 +4362,10 @@
     </row>
     <row r="13" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>4</v>
@@ -4382,10 +4386,10 @@
         <v>4</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>4</v>
@@ -4429,10 +4433,10 @@
     </row>
     <row r="14" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>4</v>
@@ -4506,10 +4510,10 @@
     </row>
     <row r="15" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>4</v>
@@ -4583,10 +4587,10 @@
     </row>
     <row r="16" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>4</v>
@@ -4598,7 +4602,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>4</v>
@@ -4660,10 +4664,10 @@
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>4</v>
@@ -4675,7 +4679,7 @@
         <v>4</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>4</v>
@@ -4737,10 +4741,10 @@
     </row>
     <row r="18" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>4</v>
@@ -4752,7 +4756,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>4</v>
@@ -4814,10 +4818,10 @@
     </row>
     <row r="19" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -4829,7 +4833,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>4</v>
@@ -4891,10 +4895,10 @@
     </row>
     <row r="20" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
@@ -4906,7 +4910,7 @@
         <v>4</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>4</v>
@@ -4968,10 +4972,10 @@
     </row>
     <row r="21" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>4</v>
@@ -5045,7 +5049,7 @@
     </row>
     <row r="22" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
@@ -10052,13 +10056,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B1" s="3">
         <v>20191212</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
@@ -10066,13 +10070,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B2" s="3">
         <v>20191205</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
about done with strip down for ConsoleTest...
</commit_message>
<xml_diff>
--- a/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
+++ b/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
@@ -2412,13 +2412,6 @@
 Connect the 12-pin MTA to console.
 Connect the 4-pin MTA to the console.
 Click OK.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">将EQW1001的一端连接到EQF1259（TRED1）。注意：确保您选择匹配控制台类型的正确端口。
-将接地线（绿色）连接到EQF 1259的E-GND。
-Connect one end of the EQW1001 to EQF1259 (TRED1). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
-Connect the ground wire (Green) to E-GND on EQF 1259. 
-</t>
   </si>
   <si>
     <t xml:space="preserve">将EQW1025的一端连接到EQF1259（TRED2）。注意：确保您选择匹配控制台类型的正确端口。
@@ -3133,6 +3126,12 @@
 EQF1259 Console Fixture
 PC w/ Access to RNDftp
 MicroSD Card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">将EQW1001的一端连接到EQF1259（TRED1）。注意：确保您选择匹配控制台类型的正确端口。
+将接地线（绿色）连接到EQF 1259的E-GND。
+Connect one end of the EQW1001 to EQF1259 (TRED1). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
+Connect the ground wire (Green) to E-GND on EQF 1259. </t>
   </si>
 </sst>
 </file>
@@ -3505,7 +3504,7 @@
   <dimension ref="A1:AA70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3518,7 +3517,7 @@
         <v>349</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>350</v>
@@ -3596,13 +3595,13 @@
     </row>
     <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>330</v>
@@ -3617,19 +3616,19 @@
         <v>333</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>334</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>336</v>
@@ -3644,16 +3643,16 @@
         <v>340</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>345</v>
@@ -3665,18 +3664,18 @@
         <v>4</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>4</v>
@@ -3691,19 +3690,19 @@
         <v>4</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>414</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>415</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>338</v>
@@ -3715,16 +3714,16 @@
         <v>4</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>341</v>
@@ -3744,10 +3743,10 @@
     </row>
     <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -3768,22 +3767,22 @@
         <v>4</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>4</v>
@@ -3800,10 +3799,10 @@
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>4</v>
@@ -3824,25 +3823,25 @@
         <v>4</v>
       </c>
       <c r="I5" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>417</v>
-      </c>
       <c r="K5" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="L5" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>421</v>
-      </c>
       <c r="R5" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>4</v>
@@ -3862,10 +3861,10 @@
     </row>
     <row r="6" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>4</v>
@@ -3886,25 +3885,25 @@
         <v>4</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="M6" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>442</v>
-      </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="P6" s="5" t="s">
-        <v>446</v>
-      </c>
       <c r="R6" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>4</v>
@@ -3930,10 +3929,10 @@
     </row>
     <row r="7" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -3954,13 +3953,13 @@
         <v>4</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>4</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>4</v>
@@ -3998,10 +3997,10 @@
     </row>
     <row r="8" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -4022,10 +4021,10 @@
         <v>4</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>335</v>
@@ -4069,10 +4068,10 @@
     </row>
     <row r="9" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -4093,13 +4092,13 @@
         <v>4</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>4</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>4</v>
@@ -4146,7 +4145,7 @@
         <v>319</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -4167,7 +4166,7 @@
         <v>4</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M10" s="5" t="s">
         <v>4</v>
@@ -4211,10 +4210,10 @@
     </row>
     <row r="11" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
@@ -4226,7 +4225,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>4</v>
@@ -4235,10 +4234,10 @@
         <v>4</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>371</v>
@@ -4288,7 +4287,7 @@
         <v>320</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>4</v>
@@ -4365,7 +4364,7 @@
         <v>321</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>4</v>
@@ -4386,10 +4385,10 @@
         <v>4</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>4</v>
@@ -4436,7 +4435,7 @@
         <v>322</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>4</v>
@@ -4513,7 +4512,7 @@
         <v>323</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>4</v>
@@ -4590,7 +4589,7 @@
         <v>324</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>4</v>
@@ -4667,7 +4666,7 @@
         <v>325</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>4</v>
@@ -4744,7 +4743,7 @@
         <v>326</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>4</v>
@@ -4821,7 +4820,7 @@
         <v>327</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -4833,7 +4832,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>4</v>
@@ -4898,7 +4897,7 @@
         <v>328</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
@@ -4975,7 +4974,7 @@
         <v>329</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>4</v>
@@ -5049,7 +5048,7 @@
     </row>
     <row r="22" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>4</v>
@@ -10056,13 +10055,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B1" s="3">
         <v>20191212</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
only commit to master...ever
</commit_message>
<xml_diff>
--- a/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
+++ b/Projects/1259_usbComm/specsheetsConsole/Sheets/ConsoleProceduresLabView.xlsx
@@ -2827,20 +2827,6 @@
 On the USB tester, Blue output current is ~2500mA.</t>
   </si>
   <si>
-    <t>触摸屏幕右下角的用户个人资料图标，清除缓存。
-触摸设置。
-触摸维护。
-轻触[清除应用程式快取]，然后选取[是]，就会出现[欢迎使用]。
-等待10秒钟，然后在EQF1259上关闭控制台电源。
-断开控制台上的所有电线和电缆。
-Clear cache by touch the user profile icon on lower right of the screen.
-Touch Settings.
-Touch Maintainance.
-Touch Clear App Cache and select YES and WELCOME will appear on display.
-Wait 10 seconds and then on the EQF1259, turn off the Console power.
-Disconnect all wires and cables from the console.</t>
-  </si>
-  <si>
     <t>Rev15</t>
   </si>
   <si>
@@ -3132,6 +3118,21 @@
 将接地线（绿色）连接到EQF 1259的E-GND。
 Connect one end of the EQW1001 to EQF1259 (TRED1). NOTE: MAKE SURE YOU SELECT THE CORRECT PORT THAT MATCH THE TYPE OF THE CONSOLE.   
 Connect the ground wire (Green) to E-GND on EQF 1259. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">在控制台上，触摸屏幕左上方的用户个人资料图标。
+触摸设置。
+触摸维护。
+轻触[清除应用程式资料]，然后选择[是]，就会出现[欢迎使用]。
+等待10秒钟，然后在EQF1259上关闭控制台电源。
+断开控制台上的所有电线和电缆。
+On the console, touch the user profile icon on the upper left of the screen.
+Touch Settings.
+Touch Maintenance.
+Touch Clear App Data and select YES and WELCOME will appear on display.
+Wait 10 seconds and then on the EQF1259, turn off the Console power.
+Disconnect all wires and cables from the console.
+</t>
   </si>
 </sst>
 </file>
@@ -3503,8 +3504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3517,7 +3518,7 @@
         <v>349</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>350</v>
@@ -3595,10 +3596,10 @@
     </row>
     <row r="2" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>463</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>464</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>465</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>404</v>
@@ -3616,7 +3617,7 @@
         <v>333</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>417</v>
@@ -3628,7 +3629,7 @@
         <v>334</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>336</v>
@@ -3646,13 +3647,13 @@
         <v>427</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>345</v>
@@ -3664,12 +3665,12 @@
         <v>4</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>429</v>
+        <v>465</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>384</v>
@@ -3690,7 +3691,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>410</v>
@@ -3717,13 +3718,13 @@
         <v>428</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>341</v>
@@ -3743,7 +3744,7 @@
     </row>
     <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>385</v>
@@ -3773,16 +3774,16 @@
         <v>4</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T4" s="5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="V4" s="5" t="s">
         <v>4</v>
@@ -3799,7 +3800,7 @@
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>387</v>
@@ -3835,13 +3836,13 @@
         <v>420</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>4</v>
@@ -3861,7 +3862,7 @@
     </row>
     <row r="6" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>388</v>
@@ -3891,19 +3892,19 @@
         <v>424</v>
       </c>
       <c r="M6" s="5" t="s">
+        <v>442</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="O6" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="N6" s="5" t="s">
-        <v>441</v>
-      </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="P6" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="R6" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>4</v>
@@ -3929,7 +3930,7 @@
     </row>
     <row r="7" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>399</v>
@@ -3959,7 +3960,7 @@
         <v>4</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>4</v>
@@ -3997,7 +3998,7 @@
     </row>
     <row r="8" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>389</v>
@@ -4068,7 +4069,7 @@
     </row>
     <row r="9" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>390</v>
@@ -4225,7 +4226,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>4</v>
@@ -4385,7 +4386,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K13" s="5" t="s">
         <v>426</v>
@@ -4820,7 +4821,7 @@
         <v>327</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>4</v>
@@ -4832,7 +4833,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>4</v>
@@ -10055,13 +10056,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B1" s="3">
         <v>20191212</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>

</xml_diff>